<commit_message>
fixing pointload, optimising profil
</commit_message>
<xml_diff>
--- a/tabellen/Tabelle_Kantholz.xlsx
+++ b/tabellen/Tabelle_Kantholz.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joelm\OneDrive\Desktop\projectbeaverdam\Bachelorarbeit B4 Trako Joel Manolias 406534\Code_B_T\tabellen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0A22A6A-B7D3-4A80-A47F-139E3BDC06FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B60EF256-7A71-43E2-9CA6-A82D8B92C882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{CC272A4F-76D5-4A80-9AEC-BBB9E5F21186}"/>
   </bookViews>
@@ -101,9 +101,6 @@
     <t>400</t>
   </si>
   <si>
-    <t>46</t>
-  </si>
-  <si>
     <t>W</t>
   </si>
   <si>
@@ -573,6 +570,9 @@
   </si>
   <si>
     <t>1372</t>
+  </si>
+  <si>
+    <t>560</t>
   </si>
 </sst>
 </file>
@@ -927,8 +927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBD924F5-F88E-42EF-BE9F-68A0FBD13D93}">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J52" sqref="J52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -963,10 +963,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -980,10 +980,10 @@
         <v>36</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>4</v>
@@ -1000,10 +1000,10 @@
         <v>48</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>5</v>
@@ -1020,13 +1020,13 @@
         <v>60</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -1040,13 +1040,13 @@
         <v>72</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -1060,13 +1060,13 @@
         <v>84</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -1080,13 +1080,13 @@
         <v>64</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -1100,13 +1100,13 @@
         <v>80</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
@@ -1120,13 +1120,13 @@
         <v>96</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -1140,13 +1140,13 @@
         <v>112</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
@@ -1160,13 +1160,13 @@
         <v>128</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="F11" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -1180,13 +1180,13 @@
         <v>144</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -1200,13 +1200,13 @@
         <v>160</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
@@ -1223,10 +1223,10 @@
         <v>6</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
@@ -1240,13 +1240,13 @@
         <v>120</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
@@ -1260,13 +1260,13 @@
         <v>140</v>
       </c>
       <c r="D16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
@@ -1280,13 +1280,13 @@
         <v>160</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
@@ -1300,13 +1300,13 @@
         <v>180</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
@@ -1320,13 +1320,13 @@
         <v>200</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
@@ -1340,13 +1340,13 @@
         <v>220</v>
       </c>
       <c r="D20" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
@@ -1360,13 +1360,13 @@
         <v>144</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E21" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
@@ -1380,13 +1380,13 @@
         <v>168</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E22" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
@@ -1400,13 +1400,13 @@
         <v>192</v>
       </c>
       <c r="D23" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
@@ -1420,13 +1420,13 @@
         <v>216</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E24" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
@@ -1440,13 +1440,13 @@
         <v>240</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E25" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
@@ -1460,13 +1460,13 @@
         <v>264</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E26" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
@@ -1480,13 +1480,13 @@
         <v>288</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
@@ -1500,13 +1500,13 @@
         <v>312</v>
       </c>
       <c r="D28" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
@@ -1520,13 +1520,13 @@
         <v>208</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E29" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F29" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
@@ -1540,13 +1540,13 @@
         <v>234</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E30" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
@@ -1560,13 +1560,13 @@
         <v>196</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E31" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
@@ -1580,13 +1580,13 @@
         <v>224</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E32" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F32" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
@@ -1600,13 +1600,13 @@
         <v>252</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E33" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F33" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
@@ -1620,13 +1620,13 @@
         <v>280</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E34" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F34" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
@@ -1640,13 +1640,13 @@
         <v>308</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E35" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F35" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
@@ -1660,13 +1660,13 @@
         <v>336</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E36" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F36" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
@@ -1680,13 +1680,13 @@
         <v>364</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E37" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F37" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
@@ -1700,13 +1700,13 @@
         <v>392</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
@@ -1720,13 +1720,13 @@
         <v>256</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E39" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F39" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
@@ -1740,13 +1740,13 @@
         <v>288</v>
       </c>
       <c r="D40" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E40" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E40" s="1" t="s">
-        <v>107</v>
-      </c>
       <c r="F40" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
@@ -1760,13 +1760,13 @@
         <v>320</v>
       </c>
       <c r="D41" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="F41" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
@@ -1780,13 +1780,13 @@
         <v>352</v>
       </c>
       <c r="D42" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E42" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="F42" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
@@ -1803,10 +1803,10 @@
         <v>7</v>
       </c>
       <c r="E43" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F43" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.35">
@@ -1823,10 +1823,10 @@
         <v>8</v>
       </c>
       <c r="E44" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F44" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.35">
@@ -1840,13 +1840,13 @@
         <v>448</v>
       </c>
       <c r="D45" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E45" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="F45" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
@@ -1860,13 +1860,13 @@
         <v>480</v>
       </c>
       <c r="D46" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E46" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="F46" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
@@ -1880,13 +1880,13 @@
         <v>324</v>
       </c>
       <c r="D47" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E47" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="F47" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.35">
@@ -1900,13 +1900,13 @@
         <v>360</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.35">
@@ -1920,13 +1920,13 @@
         <v>19</v>
       </c>
       <c r="D49" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E49" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="F49" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.35">
@@ -1940,13 +1940,13 @@
         <v>432</v>
       </c>
       <c r="D50" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E50" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E50" s="1" t="s">
-        <v>133</v>
-      </c>
       <c r="F50" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.35">
@@ -1963,10 +1963,10 @@
         <v>9</v>
       </c>
       <c r="E51" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F51" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
@@ -1983,10 +1983,10 @@
         <v>10</v>
       </c>
       <c r="E52" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F52" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.35">
@@ -2003,10 +2003,10 @@
         <v>11</v>
       </c>
       <c r="E53" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F53" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.35">
@@ -2020,13 +2020,13 @@
         <v>20</v>
       </c>
       <c r="D54" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E54" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="E54" s="1" t="s">
+      <c r="F54" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.35">
@@ -2040,13 +2040,13 @@
         <v>440</v>
       </c>
       <c r="D55" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E55" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="E55" s="1" t="s">
+      <c r="F55" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.35">
@@ -2060,13 +2060,13 @@
         <v>480</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E56" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F56" s="1" t="s">
         <v>146</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.35">
@@ -2080,13 +2080,13 @@
         <v>520</v>
       </c>
       <c r="D57" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E57" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="E57" s="1" t="s">
+      <c r="F57" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
@@ -2097,16 +2097,16 @@
         <v>28</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>21</v>
+        <v>178</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E58" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="F58" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.35">
@@ -2123,10 +2123,10 @@
         <v>4</v>
       </c>
       <c r="E59" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F59" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.35">
@@ -2143,7 +2143,7 @@
         <v>13</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F60" s="1" t="s">
         <v>17</v>
@@ -2160,13 +2160,13 @@
         <v>15</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>